<commit_message>
added the code and PPT of fast pwm using timer0
</commit_message>
<xml_diff>
--- a/Presentations/timer 0 Count calculator.xlsx
+++ b/Presentations/timer 0 Count calculator.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{D7173A68-1240-4D9E-9956-F4F26F615181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{565208BB-7A20-49C1-BEA9-F27FB58655BC}"/>
+    <workbookView minimized="1" xWindow="2340" yWindow="2100" windowWidth="10680" windowHeight="10212" xr2:uid="{565208BB-7A20-49C1-BEA9-F27FB58655BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -406,7 +406,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>